<commit_message>
doc: Added tile expansion to user stories
</commit_message>
<xml_diff>
--- a/documentation/user stories.xlsx
+++ b/documentation/user stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\WORK\UNIVERSITY\idle-theme-park-world\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C053CA-29DA-4C25-BACB-B35B50C5FA7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C27088-D921-4B3F-AEA8-4B8E3A11C4BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1D1440B7-7BEF-4BCA-9192-687B1F4C4424}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="63">
   <si>
     <t>AS A</t>
   </si>
@@ -201,19 +201,45 @@
   </si>
   <si>
     <t>The run is saved on the leaderboards if it's in the top 10</t>
+  </si>
+  <si>
+    <t>buy new fields</t>
+  </si>
+  <si>
+    <t>new field menu chosen </t>
+  </si>
+  <si>
+    <t>have enough money </t>
+  </si>
+  <si>
+    <t>the field is added </t>
+  </si>
+  <si>
+    <t>new field menu chosen  </t>
+  </si>
+  <si>
+    <t>don’t have enough money </t>
+  </si>
+  <si>
+    <t>the program says, not enough money, and returns to the menu </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -224,7 +250,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -381,15 +407,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -411,6 +428,60 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -419,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -437,6 +508,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -446,24 +526,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -779,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB75BCA-4491-406E-B4C9-5F6C6146270B}">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,729 +887,808 @@
     <col min="7" max="7" width="58.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="1" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+    <row r="12" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="6" t="s">
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="8" t="s">
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14"/>
+      <c r="B14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+    <row r="15" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
         <v>2</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="B15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="6" t="s">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="8" t="s">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>3</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="7" t="s">
+    <row r="18" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>3</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="6" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="8" t="s">
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14"/>
+      <c r="B20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+    <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="1" t="s">
+      <c r="B22" s="10"/>
+      <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="3" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+    <row r="24" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
         <v>1</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="B24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="6" t="s">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="8" t="s">
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
+      <c r="B26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+    <row r="27" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
         <v>2</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="B27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="6" t="s">
+    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
-      <c r="B21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="8" t="s">
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14"/>
+      <c r="B29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
-        <v>3</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="7" t="s">
+    <row r="30" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12">
+        <v>3</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="6" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="8" t="s">
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14"/>
+      <c r="B32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+    <row r="33" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="1" t="s">
+      <c r="B34" s="10"/>
+      <c r="C34" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
+    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="3" t="s">
+      <c r="B35" s="11"/>
+      <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+    <row r="36" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12">
         <v>1</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="7" t="s">
+      <c r="B36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="6" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="8" t="s">
+    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14"/>
+      <c r="B38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+    <row r="39" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
         <v>2</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="7" t="s">
+      <c r="B39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="6" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="11"/>
-      <c r="B33" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="8" t="s">
+    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="14"/>
+      <c r="B41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
-        <v>3</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="7" t="s">
+    <row r="42" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12">
+        <v>3</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="6" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="11"/>
-      <c r="B36" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="8" t="s">
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="14"/>
+      <c r="B44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
-        <v>4</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="7" t="s">
+    <row r="45" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12">
+        <v>4</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="6" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="11"/>
-      <c r="B39" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="8" t="s">
+    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="14"/>
+      <c r="B47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
-        <v>5</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" s="7" t="s">
+    <row r="48" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="12">
+        <v>5</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="6" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="13"/>
+      <c r="B49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="11"/>
-      <c r="B42" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="8" t="s">
+    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="14"/>
+      <c r="B50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+    <row r="51" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="12">
         <v>6</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="7" t="s">
+      <c r="B51" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="B44" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="6" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="11"/>
-      <c r="B45" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="8" t="s">
+    <row r="53" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="14"/>
+      <c r="B53" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
+    <row r="54" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="12"/>
-      <c r="C47" s="1" t="s">
+      <c r="B55" s="10"/>
+      <c r="C55" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="13" t="s">
+    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="13"/>
-      <c r="C48" s="3" t="s">
+      <c r="B56" s="11"/>
+      <c r="C56" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="9">
+    <row r="57" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="12">
         <v>1</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="7" t="s">
+      <c r="B57" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="10"/>
-      <c r="B50" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50" s="6" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="11"/>
-      <c r="B51" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="8" t="s">
+    <row r="59" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="14"/>
+      <c r="B59" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
+    <row r="60" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="12">
         <v>2</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52" s="7" t="s">
+      <c r="B60" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
-      <c r="B53" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53" s="6" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="13"/>
+      <c r="B61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="11"/>
-      <c r="B54" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="8" t="s">
+    <row r="62" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="14"/>
+      <c r="B62" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
+    <row r="63" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B56" s="12"/>
-      <c r="C56" s="1" t="s">
+      <c r="B64" s="10"/>
+      <c r="C64" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="13" t="s">
+    <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="13"/>
-      <c r="C57" s="3" t="s">
+      <c r="B65" s="11"/>
+      <c r="C65" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="9">
+    <row r="66" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="12">
         <v>1</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C58" s="7" t="s">
+      <c r="B66" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="10"/>
-      <c r="B59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C59" s="6" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="11"/>
-      <c r="B60" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="8" t="s">
+    <row r="68" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="14"/>
+      <c r="B68" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="9">
+    <row r="69" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="12">
         <v>2</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C61" s="7" t="s">
+      <c r="B69" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="10"/>
-      <c r="B62" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62" s="6" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="11"/>
-      <c r="B63" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" s="8" t="s">
+    <row r="71" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="14"/>
+      <c r="B71" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="12" t="s">
+    <row r="72" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B65" s="12"/>
-      <c r="C65" s="1" t="s">
+      <c r="B73" s="10"/>
+      <c r="C73" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="13" t="s">
+    <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B66" s="13"/>
-      <c r="C66" s="3" t="s">
+      <c r="B74" s="11"/>
+      <c r="C74" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="9">
+    <row r="75" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="12">
         <v>1</v>
       </c>
-      <c r="B67" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C67" s="7" t="s">
+      <c r="B75" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="10"/>
-      <c r="B68" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68" s="6" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="13"/>
+      <c r="B76" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="11"/>
-      <c r="B69" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="8" t="s">
+    <row r="77" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="14"/>
+      <c r="B77" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="12" t="s">
+    <row r="78" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B71" s="12"/>
-      <c r="C71" s="1" t="s">
+      <c r="B79" s="10"/>
+      <c r="C79" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="13" t="s">
+    <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B72" s="13"/>
-      <c r="C72" s="3" t="s">
+      <c r="B80" s="11"/>
+      <c r="C80" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="9">
+    <row r="81" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="12">
         <v>1</v>
       </c>
-      <c r="B73" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C73" s="7" t="s">
+      <c r="B81" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="10"/>
-      <c r="B74" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C74" s="6" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="13"/>
+      <c r="B82" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="11"/>
-      <c r="B75" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="8" t="s">
+    <row r="83" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="14"/>
+      <c r="B83" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="9">
+    <row r="84" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="12">
         <v>2</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C76" s="7" t="s">
+      <c r="B84" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="10"/>
-      <c r="B77" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C77" s="6" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="13"/>
+      <c r="B85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="11"/>
-      <c r="B78" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="8" t="s">
+    <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="14"/>
+      <c r="B86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:A54"/>
+  <mergeCells count="35">
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A55:B55"/>
     <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A34:B34"/>
     <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:A69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
doc: Adjusted user stories of speed and added pavement to UML
</commit_message>
<xml_diff>
--- a/documentation/user stories.xlsx
+++ b/documentation/user stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\WORK\UNIVERSITY\idle-theme-park-world\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C27088-D921-4B3F-AEA8-4B8E3A11C4BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D12F2EF-5870-4315-8F2C-B321705FF0AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1D1440B7-7BEF-4BCA-9192-687B1F4C4424}"/>
   </bookViews>
@@ -74,9 +74,6 @@
     <t>the current speed is above 0.5x</t>
   </si>
   <si>
-    <t>the simulation speed lowers by 0.1x</t>
-  </si>
-  <si>
     <t>the current speed is 0.5x</t>
   </si>
   <si>
@@ -89,15 +86,6 @@
     <t>I clicked the speedup button</t>
   </si>
   <si>
-    <t>the current speed is above 4x</t>
-  </si>
-  <si>
-    <t>the current speed is 4x</t>
-  </si>
-  <si>
-    <t>the simulation speed goes up by 1x</t>
-  </si>
-  <si>
     <t>I clicked the pause button in between the speed change buttons</t>
   </si>
   <si>
@@ -161,27 +149,6 @@
     <t>a window pops up showing how many are in line, current condition, total income and other statistics (plus the upgrade button)</t>
   </si>
   <si>
-    <t>build a new road</t>
-  </si>
-  <si>
-    <t>I clicked the build button and chose a road tile</t>
-  </si>
-  <si>
-    <t>hovering over a tile next to the entrance/another road tile and have enough money</t>
-  </si>
-  <si>
-    <t>hovering over a tile not next to the entrance/another road tile or not having enough money</t>
-  </si>
-  <si>
-    <t>a new road tile is placed into the play area</t>
-  </si>
-  <si>
-    <t>hovering over a base tile where the building would not be in conflict with other tiles and would be next to the entrance/another road tile with enough money</t>
-  </si>
-  <si>
-    <t>hovering over a base tile not next to the entrance/another road tile or not having enough money or having conflicts with already occupied tiles</t>
-  </si>
-  <si>
     <t>register a run on the leaderboards</t>
   </si>
   <si>
@@ -222,6 +189,39 @@
   </si>
   <si>
     <t>the program says, not enough money, and returns to the menu </t>
+  </si>
+  <si>
+    <t>build a new pavement</t>
+  </si>
+  <si>
+    <t>I clicked the build button and chose a pavement tile</t>
+  </si>
+  <si>
+    <t>hovering over a tile next to the entrance/another pavement tile and have enough money</t>
+  </si>
+  <si>
+    <t>hovering over a tile not next to the entrance/another pavement tile or not having enough money</t>
+  </si>
+  <si>
+    <t>a new pavement tile is placed into the play area</t>
+  </si>
+  <si>
+    <t>hovering over a base tile where the building would not be in conflict with other tiles and would be next to the entrance/another pavement tile with enough money</t>
+  </si>
+  <si>
+    <t>hovering over a base tile not next to the entrance/another pavement tile or not having enough money or having conflicts with already occupied tiles</t>
+  </si>
+  <si>
+    <t>the simulation speed slows down (from 1x to 0.5x and 2x to 1x)</t>
+  </si>
+  <si>
+    <t>the current speed is below 2x</t>
+  </si>
+  <si>
+    <t>the simulation speed speeds up (from 0.5x to 1x and 1x to 2x)</t>
+  </si>
+  <si>
+    <t>the current speed is 2x</t>
   </si>
 </sst>
 </file>
@@ -250,7 +250,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -436,47 +436,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thick">
         <color indexed="64"/>
       </right>
@@ -490,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -511,27 +470,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -542,19 +480,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -873,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB75BCA-4491-406E-B4C9-5F6C6146270B}">
   <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,10 +841,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="20"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -902,77 +855,77 @@
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>57</v>
+      <c r="C3" s="14" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>58</v>
+      <c r="C4" s="15" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+      <c r="C5" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
+      <c r="C6" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>61</v>
+      <c r="C7" s="15" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>62</v>
+      <c r="C8" s="23" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
@@ -983,31 +936,31 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="3" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="16">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
@@ -1016,27 +969,27 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="16">
         <v>2</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
@@ -1045,18 +998,18 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="A18" s="16">
         <v>3</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1065,35 +1018,35 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="10"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="11"/>
+      <c r="B23" s="22"/>
       <c r="C23" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
+      <c r="A24" s="16">
         <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1104,16 +1057,16 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="5" t="s">
         <v>5</v>
       </c>
@@ -1122,7 +1075,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
+      <c r="A27" s="16">
         <v>2</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -1133,16 +1086,16 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="5" t="s">
         <v>5</v>
       </c>
@@ -1151,7 +1104,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12">
+      <c r="A30" s="16">
         <v>3</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -1162,7 +1115,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="1" t="s">
         <v>4</v>
       </c>
@@ -1171,46 +1124,46 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="10"/>
+      <c r="B34" s="21"/>
       <c r="C34" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="11"/>
+      <c r="B35" s="22"/>
       <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12">
+      <c r="A36" s="16">
         <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
+      <c r="A37" s="17"/>
       <c r="B37" s="1" t="s">
         <v>4</v>
       </c>
@@ -1219,441 +1172,460 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="16">
+        <v>2</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
+      <c r="B40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="12">
-        <v>2</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="7" t="s">
+    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="18"/>
+      <c r="B41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="16">
+        <v>3</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="6" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="17"/>
+      <c r="B43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="18"/>
+      <c r="B44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="16">
+        <v>4</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="17"/>
+      <c r="B46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="18"/>
+      <c r="B47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="14"/>
-      <c r="B41" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="12">
-        <v>3</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="7" t="s">
+    <row r="48" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="16">
+        <v>5</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="6" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="17"/>
+      <c r="B49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="14"/>
-      <c r="B44" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="8" t="s">
+    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="18"/>
+      <c r="B50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="16">
+        <v>6</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="17"/>
+      <c r="B52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="12">
-        <v>4</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="14"/>
-      <c r="B47" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="12">
-        <v>5</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="7" t="s">
+    <row r="53" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="18"/>
+      <c r="B53" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="14"/>
-      <c r="B50" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="12">
-        <v>6</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="14"/>
-      <c r="B53" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B55" s="10"/>
+      <c r="B55" s="21"/>
       <c r="C55" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B56" s="11"/>
+      <c r="B56" s="22"/>
       <c r="C56" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="16">
+        <v>1</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="17"/>
+      <c r="B58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="18"/>
+      <c r="B59" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="16">
+        <v>2</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="17"/>
+      <c r="B61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="18"/>
+      <c r="B62" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="12">
-        <v>1</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="14"/>
-      <c r="B59" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="12">
-        <v>2</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="14"/>
-      <c r="B62" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B64" s="10"/>
+      <c r="B64" s="21"/>
       <c r="C64" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B65" s="11"/>
+      <c r="B65" s="22"/>
       <c r="C65" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="12">
+      <c r="A66" s="16">
         <v>1</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C66" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="17"/>
+      <c r="B67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="18"/>
+      <c r="B68" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
-      <c r="B67" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C67" s="6" t="s">
+    <row r="69" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="16">
+        <v>2</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="17"/>
+      <c r="B70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="18"/>
+      <c r="B71" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="8" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="14"/>
-      <c r="B68" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="12">
-        <v>2</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
-      <c r="B70" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="14"/>
-      <c r="B71" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
+      <c r="A73" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B73" s="10"/>
+      <c r="B73" s="21"/>
       <c r="C73" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="11" t="s">
+      <c r="A74" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B74" s="11"/>
+      <c r="B74" s="22"/>
       <c r="C74" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="12">
+      <c r="A75" s="16">
         <v>1</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="13"/>
+      <c r="A76" s="17"/>
       <c r="B76" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="14"/>
+      <c r="A77" s="18"/>
       <c r="B77" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="10" t="s">
+      <c r="A79" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B79" s="10"/>
+      <c r="B79" s="21"/>
       <c r="C79" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="11"/>
+      <c r="B80" s="22"/>
       <c r="C80" s="3" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="12">
+      <c r="A81" s="16">
         <v>1</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="13"/>
+      <c r="A82" s="17"/>
       <c r="B82" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="14"/>
+      <c r="A83" s="18"/>
       <c r="B83" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="12">
+      <c r="A84" s="16">
         <v>2</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="13"/>
+      <c r="A85" s="17"/>
       <c r="B85" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="14"/>
+      <c r="A86" s="18"/>
       <c r="B86" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
     <mergeCell ref="A75:A77"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:A5"/>
@@ -1670,25 +1642,6 @@
     <mergeCell ref="A60:A62"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="A84:A86"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A65:B65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
doc: Added pdf version of user stories
</commit_message>
<xml_diff>
--- a/documentation/user stories.xlsx
+++ b/documentation/user stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\WORK\UNIVERSITY\idle-theme-park-world\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D12F2EF-5870-4315-8F2C-B321705FF0AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFC2210-5FF0-431E-895C-9502FC7FD9F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1D1440B7-7BEF-4BCA-9192-687B1F4C4424}"/>
   </bookViews>
@@ -486,6 +486,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -501,14 +504,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -827,7 +827,7 @@
   <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,10 +841,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -859,7 +859,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="A3" s="17">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -870,7 +870,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -879,7 +879,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
@@ -888,8 +888,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
-        <v>1</v>
+      <c r="A6" s="17">
+        <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -899,7 +899,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -908,11 +908,11 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="16" t="s">
         <v>51</v>
       </c>
     </row>
@@ -922,10 +922,10 @@
       <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="20"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
@@ -940,7 +940,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+      <c r="A12" s="17">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -951,7 +951,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
@@ -960,7 +960,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
@@ -969,7 +969,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
+      <c r="A15" s="17">
         <v>2</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -980,7 +980,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
@@ -989,7 +989,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
@@ -998,7 +998,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
+      <c r="A18" s="17">
         <v>3</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1009,7 +1009,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1018,7 +1018,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="5" t="s">
         <v>5</v>
       </c>
@@ -1028,10 +1028,10 @@
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="21"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
@@ -1046,7 +1046,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="16">
+      <c r="A24" s="17">
         <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1057,7 +1057,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="1" t="s">
         <v>4</v>
       </c>
@@ -1066,7 +1066,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="5" t="s">
         <v>5</v>
       </c>
@@ -1075,7 +1075,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="16">
+      <c r="A27" s="17">
         <v>2</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -1086,7 +1086,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="1" t="s">
         <v>4</v>
       </c>
@@ -1095,7 +1095,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="18"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="5" t="s">
         <v>5</v>
       </c>
@@ -1104,7 +1104,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16">
+      <c r="A30" s="17">
         <v>3</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -1115,7 +1115,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="1" t="s">
         <v>4</v>
       </c>
@@ -1124,7 +1124,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="5" t="s">
         <v>5</v>
       </c>
@@ -1134,10 +1134,10 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="21"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="1" t="s">
         <v>1</v>
       </c>
@@ -1152,7 +1152,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="16">
+      <c r="A36" s="17">
         <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -1163,7 +1163,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="1" t="s">
         <v>4</v>
       </c>
@@ -1172,7 +1172,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="5" t="s">
         <v>5</v>
       </c>
@@ -1181,7 +1181,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="16">
+      <c r="A39" s="17">
         <v>2</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -1192,7 +1192,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="1" t="s">
         <v>4</v>
       </c>
@@ -1201,7 +1201,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="18"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="5" t="s">
         <v>5</v>
       </c>
@@ -1210,7 +1210,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="16">
+      <c r="A42" s="17">
         <v>3</v>
       </c>
       <c r="B42" s="4" t="s">
@@ -1221,7 +1221,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="1" t="s">
         <v>4</v>
       </c>
@@ -1230,7 +1230,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="18"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="5" t="s">
         <v>5</v>
       </c>
@@ -1239,7 +1239,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="16">
+      <c r="A45" s="17">
         <v>4</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -1250,7 +1250,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="1" t="s">
         <v>4</v>
       </c>
@@ -1259,7 +1259,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="18"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="5" t="s">
         <v>5</v>
       </c>
@@ -1268,7 +1268,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16">
+      <c r="A48" s="17">
         <v>5</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -1279,7 +1279,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
+      <c r="A49" s="18"/>
       <c r="B49" s="1" t="s">
         <v>4</v>
       </c>
@@ -1288,7 +1288,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="18"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="5" t="s">
         <v>5</v>
       </c>
@@ -1297,7 +1297,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="16">
+      <c r="A51" s="17">
         <v>6</v>
       </c>
       <c r="B51" s="4" t="s">
@@ -1308,7 +1308,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
+      <c r="A52" s="18"/>
       <c r="B52" s="1" t="s">
         <v>4</v>
       </c>
@@ -1317,7 +1317,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="18"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="5" t="s">
         <v>5</v>
       </c>
@@ -1327,10 +1327,10 @@
     </row>
     <row r="54" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="21" t="s">
+      <c r="A55" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B55" s="21"/>
+      <c r="B55" s="23"/>
       <c r="C55" s="1" t="s">
         <v>1</v>
       </c>
@@ -1345,7 +1345,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="16">
+      <c r="A57" s="17">
         <v>1</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -1356,7 +1356,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
+      <c r="A58" s="18"/>
       <c r="B58" s="1" t="s">
         <v>4</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="18"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="5" t="s">
         <v>5</v>
       </c>
@@ -1374,7 +1374,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="16">
+      <c r="A60" s="17">
         <v>2</v>
       </c>
       <c r="B60" s="4" t="s">
@@ -1385,7 +1385,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="1" t="s">
         <v>4</v>
       </c>
@@ -1394,7 +1394,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="18"/>
+      <c r="A62" s="19"/>
       <c r="B62" s="5" t="s">
         <v>5</v>
       </c>
@@ -1404,10 +1404,10 @@
     </row>
     <row r="63" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="21" t="s">
+      <c r="A64" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B64" s="21"/>
+      <c r="B64" s="23"/>
       <c r="C64" s="1" t="s">
         <v>1</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="16">
+      <c r="A66" s="17">
         <v>1</v>
       </c>
       <c r="B66" s="4" t="s">
@@ -1433,7 +1433,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="17"/>
+      <c r="A67" s="18"/>
       <c r="B67" s="1" t="s">
         <v>4</v>
       </c>
@@ -1442,7 +1442,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="18"/>
+      <c r="A68" s="19"/>
       <c r="B68" s="5" t="s">
         <v>5</v>
       </c>
@@ -1451,7 +1451,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="16">
+      <c r="A69" s="17">
         <v>2</v>
       </c>
       <c r="B69" s="4" t="s">
@@ -1462,7 +1462,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="17"/>
+      <c r="A70" s="18"/>
       <c r="B70" s="1" t="s">
         <v>4</v>
       </c>
@@ -1471,7 +1471,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="18"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="5" t="s">
         <v>5</v>
       </c>
@@ -1481,10 +1481,10 @@
     </row>
     <row r="72" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="21" t="s">
+      <c r="A73" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B73" s="21"/>
+      <c r="B73" s="23"/>
       <c r="C73" s="1" t="s">
         <v>1</v>
       </c>
@@ -1499,7 +1499,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="16">
+      <c r="A75" s="17">
         <v>1</v>
       </c>
       <c r="B75" s="4" t="s">
@@ -1510,7 +1510,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="17"/>
+      <c r="A76" s="18"/>
       <c r="B76" s="1" t="s">
         <v>4</v>
       </c>
@@ -1519,7 +1519,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="18"/>
+      <c r="A77" s="19"/>
       <c r="B77" s="5" t="s">
         <v>5</v>
       </c>
@@ -1529,10 +1529,10 @@
     </row>
     <row r="78" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="21" t="s">
+      <c r="A79" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B79" s="21"/>
+      <c r="B79" s="23"/>
       <c r="C79" s="1" t="s">
         <v>1</v>
       </c>
@@ -1547,7 +1547,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="16">
+      <c r="A81" s="17">
         <v>1</v>
       </c>
       <c r="B81" s="4" t="s">
@@ -1558,7 +1558,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="17"/>
+      <c r="A82" s="18"/>
       <c r="B82" s="1" t="s">
         <v>4</v>
       </c>
@@ -1567,7 +1567,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="18"/>
+      <c r="A83" s="19"/>
       <c r="B83" s="5" t="s">
         <v>5</v>
       </c>
@@ -1576,7 +1576,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="16">
+      <c r="A84" s="17">
         <v>2</v>
       </c>
       <c r="B84" s="4" t="s">
@@ -1587,7 +1587,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="17"/>
+      <c r="A85" s="18"/>
       <c r="B85" s="1" t="s">
         <v>4</v>
       </c>
@@ -1596,7 +1596,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="18"/>
+      <c r="A86" s="19"/>
       <c r="B86" s="5" t="s">
         <v>5</v>
       </c>
@@ -1607,6 +1607,25 @@
     <row r="87" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:A59"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="A84:A86"/>
     <mergeCell ref="A10:B10"/>
@@ -1623,25 +1642,6 @@
     <mergeCell ref="A65:B65"/>
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A39:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adjusted user stories concerning building
</commit_message>
<xml_diff>
--- a/documentation/user stories.xlsx
+++ b/documentation/user stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\WORK\UNIVERSITY\idle-theme-park-world\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFC2210-5FF0-431E-895C-9502FC7FD9F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42267B2-931F-4D1D-9D54-EB74574CBEA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1D1440B7-7BEF-4BCA-9192-687B1F4C4424}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="64">
   <si>
     <t>AS A</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>the current speed is 2x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">find a legal building location </t>
   </si>
 </sst>
 </file>
@@ -250,7 +253,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -445,11 +448,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -498,17 +512,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -824,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB75BCA-4491-406E-B4C9-5F6C6146270B}">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,10 +862,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="23"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -922,10 +943,10 @@
       <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1028,21 +1049,21 @@
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="23"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="22"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="3" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1104,85 +1125,83 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
-        <v>3</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="7" t="s">
+      <c r="A30" s="24"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="26"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="17">
+        <v>3</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="6" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="19"/>
-      <c r="B32" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="8" t="s">
+    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="19"/>
+      <c r="B35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
+    <row r="36" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="1" t="s">
+      <c r="B37" s="23"/>
+      <c r="C37" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="22" t="s">
+    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="3" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
-        <v>1</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="19"/>
-      <c r="B38" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>3</v>
@@ -1197,7 +1216,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1206,18 +1225,18 @@
         <v>5</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1226,7 +1245,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1235,12 +1254,12 @@
         <v>5</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>3</v>
@@ -1255,7 +1274,7 @@
         <v>4</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1264,18 +1283,18 @@
         <v>5</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1284,7 +1303,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1293,12 +1312,12 @@
         <v>5</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>3</v>
@@ -1313,69 +1332,69 @@
         <v>4</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="19"/>
       <c r="B53" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="17">
+        <v>6</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="18"/>
+      <c r="B55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="19"/>
+      <c r="B56" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="23" t="s">
+    <row r="57" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B55" s="23"/>
-      <c r="C55" s="1" t="s">
+      <c r="B58" s="20"/>
+      <c r="C58" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="22" t="s">
+    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B56" s="22"/>
-      <c r="C56" s="3" t="s">
+      <c r="B59" s="21"/>
+      <c r="C59" s="3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="17">
-        <v>1</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="18"/>
-      <c r="B58" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="19"/>
-      <c r="B59" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A60" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>3</v>
@@ -1390,7 +1409,7 @@
         <v>4</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1399,60 +1418,60 @@
         <v>5</v>
       </c>
       <c r="C62" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="17">
+        <v>2</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="18"/>
+      <c r="B64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="19"/>
+      <c r="B65" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="23" t="s">
+    <row r="66" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B64" s="23"/>
-      <c r="C64" s="1" t="s">
+      <c r="B67" s="20"/>
+      <c r="C67" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="22" t="s">
+    <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B65" s="22"/>
-      <c r="C65" s="3" t="s">
+      <c r="B68" s="21"/>
+      <c r="C68" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="17">
-        <v>1</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="18"/>
-      <c r="B67" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="19"/>
-      <c r="B68" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>3</v>
@@ -1467,7 +1486,7 @@
         <v>4</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1476,114 +1495,114 @@
         <v>5</v>
       </c>
       <c r="C71" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="17">
+        <v>2</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="18"/>
+      <c r="B73" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="19"/>
+      <c r="B74" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="23" t="s">
+    <row r="75" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B73" s="23"/>
-      <c r="C73" s="1" t="s">
+      <c r="B76" s="20"/>
+      <c r="C76" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="22" t="s">
+    <row r="77" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B74" s="22"/>
-      <c r="C74" s="3" t="s">
+      <c r="B77" s="21"/>
+      <c r="C77" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="17">
+    <row r="78" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="17">
         <v>1</v>
       </c>
-      <c r="B75" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C75" s="7" t="s">
+      <c r="B78" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="18"/>
+      <c r="B79" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="18"/>
-      <c r="B76" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="19"/>
-      <c r="B77" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="8" t="s">
+    <row r="80" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="19"/>
+      <c r="B80" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="23" t="s">
+    <row r="81" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B79" s="23"/>
-      <c r="C79" s="1" t="s">
+      <c r="B82" s="20"/>
+      <c r="C82" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="22" t="s">
+    <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="22"/>
-      <c r="C80" s="3" t="s">
+      <c r="B83" s="21"/>
+      <c r="C83" s="3" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="17">
-        <v>1</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="18"/>
-      <c r="B82" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="19"/>
-      <c r="B83" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A84" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1592,44 +1611,55 @@
         <v>4</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="19"/>
       <c r="B86" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C86" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="17">
+        <v>2</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="18"/>
+      <c r="B88" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="19"/>
+      <c r="B89" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A81:A83"/>
+  <mergeCells count="37">
+    <mergeCell ref="A33:A35"/>
     <mergeCell ref="A84:A86"/>
+    <mergeCell ref="A87:A89"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A38:B38"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
@@ -1637,11 +1667,31 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A39:A41"/>
     <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A82:B82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>